<commit_message>
finding problem in 553
</commit_message>
<xml_diff>
--- a/data/Interventions.xlsx
+++ b/data/Interventions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8610e9849f4c2023/Documents/R/NCZ_Interventions/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulr\OneDrive\Documents\R\NCZ_Interventions\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{B1614184-501C-46AB-A499-93C0ECF05B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48D1DDC7-9F2B-48F7-9AB7-BCEB0403140F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D330A69-1EC1-4EBA-8A15-7C1F53C4A18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{BBB8388B-3F78-4755-8EE7-BA9B37C5CC4B}"/>
   </bookViews>
@@ -182,9 +182,6 @@
     <t xml:space="preserve">POU hot water heaters </t>
   </si>
   <si>
-    <t xml:space="preserve">Restroom DHW POU with planed refresh </t>
-  </si>
-  <si>
     <t>Heating</t>
   </si>
   <si>
@@ -204,6 +201,9 @@
   </si>
   <si>
     <t>Chiller EOL Replacement</t>
+  </si>
+  <si>
+    <t>Electrificaiton</t>
   </si>
 </sst>
 </file>
@@ -256,10 +256,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -582,7 +578,7 @@
   <dimension ref="A17:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1002,7 +998,7 @@
         <v>47</v>
       </c>
       <c r="E27" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="F27" t="s">
         <v>36</v>
@@ -1031,16 +1027,16 @@
         <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C28">
         <v>9.1999999999999993</v>
       </c>
       <c r="D28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" t="s">
         <v>50</v>
-      </c>
-      <c r="E28" t="s">
-        <v>51</v>
       </c>
       <c r="F28" t="s">
         <v>26</v>
@@ -1075,10 +1071,10 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="D29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" t="s">
         <v>52</v>
-      </c>
-      <c r="E29" t="s">
-        <v>53</v>
       </c>
       <c r="F29" t="s">
         <v>30</v>
@@ -1113,10 +1109,10 @@
         <v>9.4</v>
       </c>
       <c r="D30" t="s">
+        <v>53</v>
+      </c>
+      <c r="E30" t="s">
         <v>54</v>
-      </c>
-      <c r="E30" t="s">
-        <v>55</v>
       </c>
       <c r="F30" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
getting back into it
</commit_message>
<xml_diff>
--- a/data/Interventions.xlsx
+++ b/data/Interventions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulr\OneDrive\Documents\R\NCZ_Interventions\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8610e9849f4c2023/Documents/R/NCZ_Interventions/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D330A69-1EC1-4EBA-8A15-7C1F53C4A18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{9D330A69-1EC1-4EBA-8A15-7C1F53C4A18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85563E79-A977-4265-9BFB-436F70CBB4B0}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{BBB8388B-3F78-4755-8EE7-BA9B37C5CC4B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="54">
   <si>
     <t>Building</t>
   </si>
@@ -179,9 +179,6 @@
     <t xml:space="preserve">Rooftop solar </t>
   </si>
   <si>
-    <t xml:space="preserve">POU hot water heaters </t>
-  </si>
-  <si>
     <t>Heating</t>
   </si>
   <si>
@@ -201,9 +198,6 @@
   </si>
   <si>
     <t>Chiller EOL Replacement</t>
-  </si>
-  <si>
-    <t>Electrificaiton</t>
   </si>
 </sst>
 </file>
@@ -575,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4836DB5D-844D-4133-A937-590569F4A7CE}">
-  <dimension ref="A17:P30"/>
+  <dimension ref="A17:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -989,31 +983,31 @@
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C27">
-        <v>9.1</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="D27" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E27" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F27" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="G27">
-        <v>196000</v>
+        <v>2100000</v>
       </c>
       <c r="H27" t="s">
         <v>27</v>
       </c>
       <c r="I27">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="L27">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="M27">
         <v>2025</v>
@@ -1027,34 +1021,34 @@
         <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="C28">
-        <v>9.1999999999999993</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="D28" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E28" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F28" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G28">
-        <v>2100000</v>
+        <v>54100000</v>
       </c>
       <c r="H28" t="s">
         <v>27</v>
       </c>
       <c r="I28">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="L28">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="M28">
-        <v>2025</v>
+        <v>2035</v>
       </c>
       <c r="P28" t="s">
         <v>22</v>
@@ -1065,74 +1059,36 @@
         <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C29">
-        <v>9.3000000000000007</v>
+        <v>9.4</v>
       </c>
       <c r="D29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F29" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="G29">
-        <v>54100000</v>
+        <v>1950000</v>
       </c>
       <c r="H29" t="s">
         <v>27</v>
       </c>
       <c r="I29">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="L29">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="M29">
-        <v>2035</v>
+        <v>2030</v>
       </c>
       <c r="P29" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30" t="s">
-        <v>31</v>
-      </c>
-      <c r="C30">
-        <v>9.4</v>
-      </c>
-      <c r="D30" t="s">
-        <v>53</v>
-      </c>
-      <c r="E30" t="s">
-        <v>54</v>
-      </c>
-      <c r="F30" t="s">
-        <v>36</v>
-      </c>
-      <c r="G30">
-        <v>1950000</v>
-      </c>
-      <c r="H30" t="s">
-        <v>27</v>
-      </c>
-      <c r="I30">
-        <v>0.02</v>
-      </c>
-      <c r="L30">
-        <v>35</v>
-      </c>
-      <c r="M30">
-        <v>2030</v>
-      </c>
-      <c r="P30" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
GETTING THIS BACKINTO MY HEAD
</commit_message>
<xml_diff>
--- a/data/Interventions.xlsx
+++ b/data/Interventions.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29721"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8610e9849f4c2023/Documents/R/NCZ_Interventions/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{9D330A69-1EC1-4EBA-8A15-7C1F53C4A18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85563E79-A977-4265-9BFB-436F70CBB4B0}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{9D330A69-1EC1-4EBA-8A15-7C1F53C4A18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E6823D8-89A8-43A4-94A8-FB8A6C024009}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{BBB8388B-3F78-4755-8EE7-BA9B37C5CC4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -92,7 +92,7 @@
     <t>Heating &amp; Cooling</t>
   </si>
   <si>
-    <t>Retrocommissioning  (RCx)</t>
+    <t>Retrocommissioning  (RCx) xxxxxxxx</t>
   </si>
   <si>
     <t xml:space="preserve">Implement ECMs from ComEd report </t>
@@ -204,7 +204,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -572,15 +572,16 @@
   <dimension ref="A17:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="6" max="6" width="16.59765625" customWidth="1"/>
+    <col min="4" max="4" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:16">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -630,7 +631,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:16">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -671,7 +672,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:16">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -709,7 +710,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:16">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -750,7 +751,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:16">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -788,7 +789,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:16">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -826,7 +827,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:16">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -864,7 +865,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:16">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -902,7 +903,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:16">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -940,7 +941,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:16">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -978,7 +979,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:16">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -1016,7 +1017,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:16">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -1054,7 +1055,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:16">
       <c r="A29" t="s">
         <v>16</v>
       </c>

</xml_diff>